<commit_message>
Transaction value moved to offer_completed records and split up according to reward ratio
</commit_message>
<xml_diff>
--- a/data/starbucks_data_test.xlsx
+++ b/data/starbucks_data_test.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BA495F1-D94D-4715-9821-9BEBB0259701}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A17410-BB2F-4051-A17B-C0CDE6E36EA6}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
   </bookViews>
   <sheets>
     <sheet name="transcript" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">transcript!$A$1:$N$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">transcript!$A$1:$N$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="91">
   <si>
     <t>person</t>
   </si>
@@ -253,21 +253,74 @@
   </si>
   <si>
     <t>Transaction amount at time of offer completion related to offer</t>
+  </si>
+  <si>
+    <t>ffff82501cea40309d5fdd7edcca4a07</t>
+  </si>
+  <si>
+    <t>of_dup</t>
+  </si>
+  <si>
+    <t>{'amount': 16.06}</t>
+  </si>
+  <si>
+    <t>{'amount': 7.18}</t>
+  </si>
+  <si>
+    <t>{'amount': 9.12}</t>
+  </si>
+  <si>
+    <t>{'amount': 22.88}</t>
+  </si>
+  <si>
+    <t>{'offer_id': '0b1e1539f2cc45b7b9fa7c272da2e1d7', 'reward': 5}</t>
+  </si>
+  <si>
+    <t>{'amount': 15.23}</t>
+  </si>
+  <si>
+    <t>{'amount': 18.08}</t>
+  </si>
+  <si>
+    <t>{'amount': 23.32}</t>
+  </si>
+  <si>
+    <t>{'amount': 16.86}</t>
+  </si>
+  <si>
+    <t>{'amount': 15.57}</t>
+  </si>
+  <si>
+    <t>{'offer_id': '2906b810c7d4411798c6938adc9daaa5', 'reward': 2}</t>
+  </si>
+  <si>
+    <t>{'amount': 17.55}</t>
+  </si>
+  <si>
+    <t>{'amount': 13.17}</t>
+  </si>
+  <si>
+    <t>{'amount': 7.79}</t>
+  </si>
+  <si>
+    <t>{'amount': 14.23}</t>
+  </si>
+  <si>
+    <t>{'amount': 10.12}</t>
+  </si>
+  <si>
+    <t>{'amount': 18.91}</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Porsche Next TT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Porsche Next TT"/>
@@ -316,6 +369,32 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -383,29 +462,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,11 +806,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
@@ -745,49 +831,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -802,7 +890,7 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J2" t="s">
@@ -813,266 +901,255 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A6" s="2">
+        <v>1393</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
         <v>15561</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
-        <v>47582</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4">
-        <v>132</v>
-      </c>
-      <c r="G4">
-        <v>19.89</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
-        <v>47583</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5">
-        <v>132</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5">
-        <f>E5-E2</f>
-        <v>132</v>
-      </c>
-      <c r="L5">
-        <f>E5-E3</f>
-        <v>126</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
-        <v>49502</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6">
-        <v>144</v>
-      </c>
-      <c r="G6">
-        <v>17.78</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
-        <v>53176</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E7">
-        <v>168</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
+        <v>6</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <v>85291</v>
+      <c r="A8" s="2">
+        <v>15562</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>216</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>37</v>
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
-        <v>87134</v>
+      <c r="A9" s="2">
+        <v>15836</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E9">
-        <v>222</v>
-      </c>
-      <c r="G9">
-        <v>19.670000000000002</v>
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
-      <c r="J9" t="e">
-        <v>#N/A</v>
+      <c r="J9" t="s">
+        <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
-        <v>92104</v>
+      <c r="A10" s="2">
+        <v>20283</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>240</v>
-      </c>
-      <c r="G10">
-        <v>29.72</v>
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="J10" t="e">
-        <v>#N/A</v>
+      <c r="J10" t="s">
+        <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="3">
-        <v>141566</v>
+      <c r="A11" s="2">
+        <v>32762</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="E11">
-        <v>378</v>
+        <v>60</v>
       </c>
       <c r="G11">
-        <v>23.93</v>
+        <v>16.059999999999999</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -1081,99 +1158,102 @@
         <v>#N/A</v>
       </c>
       <c r="N11" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="3">
-        <v>150598</v>
+      <c r="A12" s="2">
+        <v>32763</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
+        <v>71</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E12">
-        <v>408</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J12" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N12" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
-        <v>163375</v>
+      <c r="A13" s="2">
+        <v>37060</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E13">
-        <v>408</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>52</v>
+        <v>78</v>
+      </c>
+      <c r="G13">
+        <v>7.18</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
       </c>
-      <c r="J13" t="s">
-        <v>13</v>
+      <c r="J13" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N13" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A14" s="3">
-        <v>201572</v>
+      <c r="A14" s="2">
+        <v>45575</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E14">
-        <v>504</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>56</v>
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <v>9.1199999999999992</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
       </c>
-      <c r="J14" t="s">
-        <v>13</v>
+      <c r="J14" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N14" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
-        <v>218393</v>
+      <c r="A15" s="2">
+        <v>47582</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -1182,13 +1262,13 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E15">
-        <v>510</v>
+        <v>132</v>
       </c>
       <c r="G15">
-        <v>21.72</v>
+        <v>19.89</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1201,26 +1281,26 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A16" s="3">
-        <v>218394</v>
+      <c r="A16" s="2">
+        <v>47583</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E16">
-        <v>510</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>52</v>
+        <v>132</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="H16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I16" t="s">
         <v>31</v>
@@ -1229,153 +1309,142 @@
         <v>13</v>
       </c>
       <c r="K16">
-        <f>E16-E12</f>
-        <v>102</v>
+        <f>E16-E13</f>
+        <v>54</v>
       </c>
       <c r="L16">
-        <f>E16-E13</f>
-        <v>102</v>
+        <f>E16-E14</f>
+        <v>12</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="3">
-        <v>218395</v>
+      <c r="A17" s="2">
+        <v>49502</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>33</v>
+      <c r="C17" t="s">
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E17">
-        <v>510</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17">
-        <v>5</v>
+        <v>144</v>
+      </c>
+      <c r="G17">
+        <v>17.78</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17">
-        <f>E17-E14</f>
-        <v>6</v>
-      </c>
-      <c r="L17">
-        <f>E17-E19</f>
-        <v>-72</v>
+        <v>18</v>
+      </c>
+      <c r="J17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A18" s="3">
-        <v>230412</v>
+      <c r="A18" s="2">
+        <v>53176</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="E18">
-        <v>534</v>
-      </c>
-      <c r="G18">
-        <v>26.56</v>
+        <v>168</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
-      <c r="J18" t="e">
-        <v>#N/A</v>
+      <c r="J18" t="s">
+        <v>28</v>
       </c>
       <c r="N18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A19" s="3">
-        <v>262138</v>
+      <c r="A19" s="2">
+        <v>53182</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E19">
-        <v>582</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>56</v>
+        <v>168</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="3">
-        <v>7</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A20" s="2">
+        <v>54574</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
       </c>
       <c r="J20" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="3">
-        <v>53182</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A21" s="2">
+        <v>65844</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
@@ -1396,24 +1465,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="3">
-        <v>65844</v>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A22" s="2">
+        <v>69626</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E22">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="I22" t="s">
         <v>18</v>
@@ -1422,27 +1491,27 @@
         <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="3">
-        <v>85293</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A23" s="2">
+        <v>79667</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="E23">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="G23">
-        <v>2.3199999999999998</v>
+        <v>22.88</v>
       </c>
       <c r="I23" t="s">
         <v>18</v>
@@ -1451,99 +1520,102 @@
         <v>#N/A</v>
       </c>
       <c r="N23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="3">
-        <v>110835</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A24" s="2">
+        <v>79668</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
+        <v>71</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="E24">
-        <v>336</v>
+        <v>198</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>17</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s">
         <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3">
-        <v>130152</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <v>81594</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25">
+        <v>204</v>
+      </c>
+      <c r="G25">
+        <v>15.23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>85291</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="D25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25">
-        <v>348</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" t="s">
-        <v>19</v>
-      </c>
-      <c r="N25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="3">
-        <v>141567</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E26">
-        <v>378</v>
-      </c>
-      <c r="G26">
-        <v>5.29</v>
+        <v>216</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I26" t="s">
         <v>18</v>
       </c>
-      <c r="J26" t="e">
-        <v>#N/A</v>
+      <c r="J26" t="s">
+        <v>28</v>
       </c>
       <c r="N26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="3">
-        <v>187136</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A27" s="2">
+        <v>85293</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -1552,13 +1624,13 @@
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E27">
-        <v>456</v>
+        <v>216</v>
       </c>
       <c r="G27">
-        <v>7.14</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="I27" t="s">
         <v>18</v>
@@ -1570,56 +1642,53 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="3">
-        <v>187137</v>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A28" s="2">
+        <v>87134</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E28">
-        <v>456</v>
-      </c>
-      <c r="F28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
+        <v>222</v>
+      </c>
+      <c r="G28">
+        <v>19.670000000000002</v>
       </c>
       <c r="I28" t="s">
-        <v>31</v>
-      </c>
-      <c r="J28" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="3">
-        <v>243231</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A29" s="2">
+        <v>90553</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="E29">
-        <v>570</v>
+        <v>234</v>
       </c>
       <c r="G29">
-        <v>0.87</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I29" t="s">
         <v>18</v>
@@ -1628,70 +1697,70 @@
         <v>#N/A</v>
       </c>
       <c r="N29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A30" s="2">
+        <v>90697</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>17</v>
+        <v>234</v>
+      </c>
+      <c r="G30">
+        <v>18.079999999999998</v>
       </c>
       <c r="I30" t="s">
         <v>18</v>
       </c>
-      <c r="J30" t="s">
-        <v>19</v>
+      <c r="J30" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="3">
-        <v>15562</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A31" s="2">
+        <v>92104</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E31">
-        <v>6</v>
-      </c>
-      <c r="F31" t="s">
-        <v>17</v>
+        <v>240</v>
+      </c>
+      <c r="G31">
+        <v>29.72</v>
       </c>
       <c r="I31" t="s">
         <v>18</v>
       </c>
-      <c r="J31" t="s">
-        <v>19</v>
+      <c r="J31" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="3">
-        <v>90553</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A32" s="2">
+        <v>97700</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
@@ -1700,13 +1769,13 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E32">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="G32">
-        <v>1.0900000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="I32" t="s">
         <v>18</v>
@@ -1718,24 +1787,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="3">
-        <v>97700</v>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A33" s="2">
+        <v>97830</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E33">
         <v>264</v>
       </c>
       <c r="G33">
-        <v>3.5</v>
+        <v>23.32</v>
       </c>
       <c r="I33" t="s">
         <v>18</v>
@@ -1744,99 +1813,99 @@
         <v>#N/A</v>
       </c>
       <c r="N33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A34" s="2">
+        <v>102635</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34">
+        <v>288</v>
+      </c>
+      <c r="G34">
+        <v>17.88</v>
+      </c>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A35" s="2">
+        <v>103834</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35">
+        <v>294</v>
+      </c>
+      <c r="G35">
+        <v>21.43</v>
+      </c>
+      <c r="I35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A36" s="2">
+        <v>107052</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36">
+        <v>312</v>
+      </c>
+      <c r="G36">
+        <v>16.86</v>
+      </c>
+      <c r="I36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A37" s="2">
         <v>110829</v>
-      </c>
-      <c r="B34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34">
-        <v>336</v>
-      </c>
-      <c r="F34" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" t="s">
-        <v>28</v>
-      </c>
-      <c r="N34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="3">
-        <v>123539</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35">
-        <v>336</v>
-      </c>
-      <c r="F35" t="s">
-        <v>27</v>
-      </c>
-      <c r="I35" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" t="s">
-        <v>28</v>
-      </c>
-      <c r="N35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="3">
-        <v>150599</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36">
-        <v>408</v>
-      </c>
-      <c r="F36" t="s">
-        <v>37</v>
-      </c>
-      <c r="I36" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" t="s">
-        <v>28</v>
-      </c>
-      <c r="N36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="3">
-        <v>201573</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
@@ -1845,100 +1914,100 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E37">
-        <v>504</v>
+        <v>336</v>
       </c>
       <c r="F37" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I37" t="s">
         <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="N37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="3">
-        <v>245125</v>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A38" s="2">
+        <v>110830</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E38">
-        <v>576</v>
+        <v>336</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I38" t="s">
         <v>18</v>
       </c>
       <c r="J38" t="s">
+        <v>28</v>
+      </c>
+      <c r="N38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A39" s="2">
+        <v>110835</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39">
+        <v>336</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" t="s">
         <v>19</v>
       </c>
-      <c r="N38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="3">
-        <v>277104</v>
-      </c>
-      <c r="B39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39">
-        <v>612</v>
-      </c>
-      <c r="G39">
-        <v>0.06</v>
-      </c>
-      <c r="I39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="3">
-        <v>281785</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A40" s="2">
+        <v>112214</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E40">
-        <v>624</v>
-      </c>
-      <c r="F40" t="s">
-        <v>17</v>
+        <v>336</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I40" t="s">
         <v>18</v>
@@ -1947,56 +2016,56 @@
         <v>19</v>
       </c>
       <c r="N40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A41" s="2">
+        <v>123539</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41">
+        <v>336</v>
+      </c>
+      <c r="F41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" t="s">
+        <v>28</v>
+      </c>
+      <c r="N41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="3">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" t="s">
-        <v>18</v>
-      </c>
-      <c r="J41" t="s">
-        <v>19</v>
-      </c>
-      <c r="N41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="3">
-        <v>20283</v>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A42" s="2">
+        <v>130152</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
         <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E42">
-        <v>18</v>
+        <v>348</v>
       </c>
       <c r="F42" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="I42" t="s">
         <v>18</v>
@@ -2005,56 +2074,56 @@
         <v>19</v>
       </c>
       <c r="N42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="3">
-        <v>102635</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A43" s="2">
+        <v>133074</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E43">
-        <v>288</v>
-      </c>
-      <c r="G43">
-        <v>17.88</v>
+        <v>354</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
       </c>
       <c r="I43" t="s">
         <v>18</v>
       </c>
-      <c r="J43" t="e">
-        <v>#N/A</v>
+      <c r="J43" t="s">
+        <v>19</v>
       </c>
       <c r="N43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="3">
-        <v>103834</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A44" s="2">
+        <v>141566</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
         <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E44">
-        <v>294</v>
+        <v>378</v>
       </c>
       <c r="G44">
-        <v>21.43</v>
+        <v>23.93</v>
       </c>
       <c r="I44" t="s">
         <v>18</v>
@@ -2063,266 +2132,1265 @@
         <v>#N/A</v>
       </c>
       <c r="N44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="3">
-        <v>110830</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
+        <v>141567</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E45">
-        <v>336</v>
-      </c>
-      <c r="F45" t="s">
-        <v>27</v>
+        <v>378</v>
+      </c>
+      <c r="G45">
+        <v>5.29</v>
       </c>
       <c r="I45" t="s">
         <v>18</v>
       </c>
-      <c r="J45" t="s">
-        <v>28</v>
+      <c r="J45" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="3">
-        <v>150600</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
+        <v>143787</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E46">
-        <v>408</v>
-      </c>
-      <c r="F46" t="s">
-        <v>12</v>
+        <v>384</v>
+      </c>
+      <c r="G46">
+        <v>15.57</v>
       </c>
       <c r="I46" t="s">
         <v>18</v>
       </c>
-      <c r="J46" t="s">
-        <v>13</v>
+      <c r="J46" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="3">
-        <v>171209</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A47" s="2">
+        <v>143788</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" t="s">
-        <v>30</v>
+        <v>71</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E47">
-        <v>420</v>
+        <v>384</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J47" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="3">
-        <v>201574</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A48" s="2">
+        <v>150598</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E48">
-        <v>504</v>
-      </c>
-      <c r="F48" t="s">
-        <v>48</v>
+        <v>408</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="I48" t="s">
         <v>18</v>
       </c>
       <c r="J48" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="3">
-        <v>225059</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A49" s="2">
+        <v>150599</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E49">
-        <v>522</v>
+        <v>408</v>
       </c>
       <c r="F49" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I49" t="s">
         <v>18</v>
       </c>
       <c r="J49" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="N49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="3">
-        <v>225060</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A50" s="2">
+        <v>150600</v>
       </c>
       <c r="B50" t="s">
         <v>21</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E50">
-        <v>522</v>
-      </c>
-      <c r="G50">
-        <v>18.420000000000002</v>
+        <v>408</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
       </c>
       <c r="I50" t="s">
         <v>18</v>
       </c>
-      <c r="J50" t="e">
-        <v>#N/A</v>
+      <c r="J50" t="s">
+        <v>13</v>
       </c>
       <c r="N50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A51" s="2">
+        <v>152030</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51">
+        <v>408</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I51" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" t="s">
+        <v>19</v>
+      </c>
+      <c r="N51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A52" s="2">
+        <v>163375</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52">
+        <v>408</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I52" t="s">
+        <v>18</v>
+      </c>
+      <c r="J52" t="s">
+        <v>13</v>
+      </c>
+      <c r="N52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A53" s="2">
+        <v>168022</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <v>414</v>
+      </c>
+      <c r="F53" t="s">
+        <v>23</v>
+      </c>
+      <c r="I53" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" t="s">
+        <v>19</v>
+      </c>
+      <c r="N53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A54" s="2">
+        <v>168023</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54">
+        <v>414</v>
+      </c>
+      <c r="G54">
+        <v>17.55</v>
+      </c>
+      <c r="I54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A55" s="2">
+        <v>168024</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55">
+        <v>414</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J55" t="s">
+        <v>19</v>
+      </c>
+      <c r="N55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A56" s="2">
+        <v>171209</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>420</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" t="s">
+        <v>13</v>
+      </c>
+      <c r="N56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A57" s="2">
+        <v>187136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57">
+        <v>456</v>
+      </c>
+      <c r="G57">
+        <v>7.14</v>
+      </c>
+      <c r="I57" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N57" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A58" s="2">
+        <v>187137</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58">
+        <v>456</v>
+      </c>
+      <c r="F58" t="s">
+        <v>48</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58" t="s">
+        <v>31</v>
+      </c>
+      <c r="J58" t="s">
+        <v>19</v>
+      </c>
+      <c r="N58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A59" s="2">
+        <v>200255</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59">
+        <v>498</v>
+      </c>
+      <c r="G59">
+        <v>13.17</v>
+      </c>
+      <c r="I59" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A60" s="2">
+        <v>201572</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>55</v>
+      </c>
+      <c r="E60">
+        <v>504</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" t="s">
+        <v>13</v>
+      </c>
+      <c r="N60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A61" s="2">
+        <v>201573</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61">
+        <v>504</v>
+      </c>
+      <c r="F61" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" t="s">
+        <v>19</v>
+      </c>
+      <c r="N61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A62" s="2">
+        <v>201574</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>47</v>
+      </c>
+      <c r="E62">
+        <v>504</v>
+      </c>
+      <c r="F62" t="s">
+        <v>48</v>
+      </c>
+      <c r="I62" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" t="s">
+        <v>19</v>
+      </c>
+      <c r="N62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A63" s="2">
+        <v>202962</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63">
+        <v>504</v>
+      </c>
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="I63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" t="s">
+        <v>13</v>
+      </c>
+      <c r="N63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A64" s="2">
+        <v>214716</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64">
+        <v>504</v>
+      </c>
+      <c r="G64">
+        <v>7.79</v>
+      </c>
+      <c r="I64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A65" s="2">
+        <v>214717</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65">
+        <v>504</v>
+      </c>
+      <c r="F65" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>31</v>
+      </c>
+      <c r="J65" t="s">
+        <v>13</v>
+      </c>
+      <c r="N65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A66" s="2">
+        <v>218393</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="10">
+        <v>510</v>
+      </c>
+      <c r="G66" s="10">
+        <v>21.72</v>
+      </c>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2">
+        <v>218394</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" s="10">
+        <v>510</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10">
+        <v>10</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K67">
+        <f>E67-E63</f>
+        <v>6</v>
+      </c>
+      <c r="L67">
+        <f>E67-E64</f>
+        <v>6</v>
+      </c>
+      <c r="N67" t="s">
+        <v>14</v>
+      </c>
+      <c r="O67">
+        <f>G66/15*10</f>
+        <v>14.48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2">
+        <v>218395</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E68" s="10">
+        <v>510</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10">
+        <v>5</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K68">
+        <f>E68-E65</f>
+        <v>6</v>
+      </c>
+      <c r="L68">
+        <f>E68-E70</f>
+        <v>-12</v>
+      </c>
+      <c r="N68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2">
+        <v>225059</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69">
+        <v>522</v>
+      </c>
+      <c r="F69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I69" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" t="s">
+        <v>19</v>
+      </c>
+      <c r="N69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A70" s="14">
+        <v>225060</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="10">
+        <v>522</v>
+      </c>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="H70" s="10"/>
+      <c r="I70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A71" s="14">
         <v>225061</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B71" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C71" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D71" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E51">
+      <c r="E71" s="10">
         <v>522</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F71" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H51">
+      <c r="G71" s="10"/>
+      <c r="H71" s="10">
         <v>5</v>
       </c>
-      <c r="I51" t="s">
-        <v>31</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="I71" t="s">
+        <v>31</v>
+      </c>
+      <c r="J71" t="s">
         <v>13</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N71" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A72" s="14">
         <v>225062</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B72" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C72" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D72" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E52">
+      <c r="E72" s="10">
         <v>522</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F72" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H52">
+      <c r="G72" s="10"/>
+      <c r="H72" s="10">
         <v>2</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I72" t="s">
         <v>33</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J72" t="s">
         <v>19</v>
       </c>
-      <c r="N52" t="s">
+      <c r="N72" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:14" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
-      <c r="K55" s="9" t="s">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2">
+        <v>230412</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73">
+        <v>534</v>
+      </c>
+      <c r="G73">
+        <v>26.56</v>
+      </c>
+      <c r="I73" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A74" s="2">
+        <v>230690</v>
+      </c>
+      <c r="B74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74">
+        <v>534</v>
+      </c>
+      <c r="F74" t="s">
+        <v>12</v>
+      </c>
+      <c r="I74" t="s">
+        <v>18</v>
+      </c>
+      <c r="J74" t="s">
+        <v>13</v>
+      </c>
+      <c r="N74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A75" s="2">
+        <v>243231</v>
+      </c>
+      <c r="B75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" t="s">
+        <v>62</v>
+      </c>
+      <c r="E75">
+        <v>570</v>
+      </c>
+      <c r="G75">
+        <v>0.87</v>
+      </c>
+      <c r="I75" t="s">
+        <v>18</v>
+      </c>
+      <c r="J75" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N75" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A76" s="2">
+        <v>245125</v>
+      </c>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76">
+        <v>576</v>
+      </c>
+      <c r="F76" t="s">
+        <v>17</v>
+      </c>
+      <c r="I76" t="s">
+        <v>18</v>
+      </c>
+      <c r="J76" t="s">
+        <v>19</v>
+      </c>
+      <c r="N76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2">
+        <v>246495</v>
+      </c>
+      <c r="B77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77">
+        <v>576</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I77" t="s">
+        <v>18</v>
+      </c>
+      <c r="J77" t="s">
+        <v>19</v>
+      </c>
+      <c r="N77" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A78" s="2">
+        <v>258361</v>
+      </c>
+      <c r="B78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78">
+        <v>576</v>
+      </c>
+      <c r="G78">
+        <v>14.23</v>
+      </c>
+      <c r="I78" t="s">
+        <v>18</v>
+      </c>
+      <c r="J78" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N78" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2">
+        <v>258362</v>
+      </c>
+      <c r="B79" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" t="s">
+        <v>83</v>
+      </c>
+      <c r="E79">
+        <v>576</v>
+      </c>
+      <c r="F79" t="s">
+        <v>23</v>
+      </c>
+      <c r="H79">
+        <v>2</v>
+      </c>
+      <c r="I79" t="s">
+        <v>31</v>
+      </c>
+      <c r="J79" t="s">
+        <v>19</v>
+      </c>
+      <c r="N79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2">
+        <v>262138</v>
+      </c>
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" t="s">
+        <v>55</v>
+      </c>
+      <c r="E80">
+        <v>582</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I80" t="s">
+        <v>18</v>
+      </c>
+      <c r="J80" t="s">
+        <v>13</v>
+      </c>
+      <c r="N80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A81" s="2">
+        <v>262475</v>
+      </c>
+      <c r="B81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" t="s">
+        <v>30</v>
+      </c>
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81">
+        <v>582</v>
+      </c>
+      <c r="F81" t="s">
+        <v>23</v>
+      </c>
+      <c r="I81" t="s">
+        <v>18</v>
+      </c>
+      <c r="J81" t="s">
+        <v>19</v>
+      </c>
+      <c r="N81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A82" s="2">
+        <v>274809</v>
+      </c>
+      <c r="B82" t="s">
+        <v>71</v>
+      </c>
+      <c r="C82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D82" t="s">
+        <v>88</v>
+      </c>
+      <c r="E82">
+        <v>606</v>
+      </c>
+      <c r="G82">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="I82" t="s">
+        <v>18</v>
+      </c>
+      <c r="J82" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A83" s="2">
+        <v>277104</v>
+      </c>
+      <c r="B83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" t="s">
+        <v>31</v>
+      </c>
+      <c r="D83" t="s">
+        <v>63</v>
+      </c>
+      <c r="E83">
+        <v>612</v>
+      </c>
+      <c r="G83">
+        <v>0.06</v>
+      </c>
+      <c r="I83" t="s">
+        <v>18</v>
+      </c>
+      <c r="J83" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A84" s="2">
+        <v>281785</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84">
+        <v>624</v>
+      </c>
+      <c r="F84" t="s">
+        <v>17</v>
+      </c>
+      <c r="I84" t="s">
+        <v>18</v>
+      </c>
+      <c r="J84" t="s">
+        <v>19</v>
+      </c>
+      <c r="N84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A85" s="2">
+        <v>289924</v>
+      </c>
+      <c r="B85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C85" t="s">
+        <v>31</v>
+      </c>
+      <c r="D85" t="s">
+        <v>89</v>
+      </c>
+      <c r="E85">
+        <v>648</v>
+      </c>
+      <c r="G85">
+        <v>18.91</v>
+      </c>
+      <c r="I85" t="s">
+        <v>18</v>
+      </c>
+      <c r="J85" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N85" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
+      <c r="K88" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="L55" s="9" t="s">
+      <c r="L88" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="M55" s="9" t="s">
+      <c r="M88" s="8" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N52" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="a"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N85" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N52">
     <sortCondition ref="N2:N52"/>
     <sortCondition ref="A2:A52"/>

</xml_diff>

<commit_message>
offer_agg prepared for enhancement by values from transcript
</commit_message>
<xml_diff>
--- a/data/starbucks_data_test.xlsx
+++ b/data/starbucks_data_test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A17410-BB2F-4051-A17B-C0CDE6E36EA6}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6578FE65-868C-4763-8E51-2068A8A7DB42}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="3420" yWindow="2115" windowWidth="27015" windowHeight="15390" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
   </bookViews>
   <sheets>
     <sheet name="transcript" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="transcript_agg" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">transcript!$A$1:$N$85</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="100">
   <si>
     <t>person</t>
   </si>
@@ -313,13 +314,40 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>offer_type</t>
+  </si>
+  <si>
+    <t>offer_duration</t>
+  </si>
+  <si>
+    <t>offer_rcvd_time</t>
+  </si>
+  <si>
+    <t>offer_difficulty</t>
+  </si>
+  <si>
+    <t>offer_reward</t>
+  </si>
+  <si>
+    <t>offer_agg</t>
+  </si>
+  <si>
+    <t>offer_viewed_time</t>
+  </si>
+  <si>
+    <t>offer_cmpl_time_el</t>
+  </si>
+  <si>
+    <t>offer_trx_amount_el</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -397,6 +425,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -462,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -492,6 +534,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,10 +853,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O67" sqref="O67"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13:G15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
   <cols>
@@ -3402,32 +3448,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E05A46-80F6-40FB-B2FF-6933C154A4AB}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>21</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neuer Ansatz Offer Aggregation Do., Mittag
</commit_message>
<xml_diff>
--- a/data/starbucks_data_test.xlsx
+++ b/data/starbucks_data_test.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6578FE65-868C-4763-8E51-2068A8A7DB42}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADC1C3F0-C74B-4355-8AC5-0F83FF9D8E5F}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
-    <workbookView xWindow="3420" yWindow="2115" windowWidth="27015" windowHeight="15390" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
+    <workbookView xWindow="-27870" yWindow="0" windowWidth="13170" windowHeight="16200" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
   </bookViews>
   <sheets>
     <sheet name="transcript" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -439,6 +439,12 @@
       <name val="Porsche Next TT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -504,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -537,6 +543,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,20 +858,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13:G15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
@@ -920,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -946,7 +954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -975,7 +983,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1004,7 +1012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>7</v>
       </c>
@@ -1033,7 +1041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>1393</v>
       </c>
@@ -1062,7 +1070,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>15561</v>
       </c>
@@ -1091,7 +1099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>15562</v>
       </c>
@@ -1120,7 +1128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>15836</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>20283</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>32762</v>
       </c>
@@ -1207,7 +1215,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>32763</v>
       </c>
@@ -1239,7 +1247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>37060</v>
       </c>
@@ -1268,7 +1276,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>45575</v>
       </c>
@@ -1297,7 +1305,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>47582</v>
       </c>
@@ -1326,7 +1334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>47583</v>
       </c>
@@ -1366,7 +1374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>49502</v>
       </c>
@@ -1395,7 +1403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>53176</v>
       </c>
@@ -1440,7 +1448,7 @@
       <c r="E19">
         <v>168</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I19" t="s">
@@ -1453,7 +1461,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>54574</v>
       </c>
@@ -1498,7 +1506,7 @@
       <c r="E21">
         <v>168</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="18" t="s">
         <v>39</v>
       </c>
       <c r="I21" t="s">
@@ -1511,7 +1519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
         <v>69626</v>
       </c>
@@ -1540,7 +1548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
         <v>79667</v>
       </c>
@@ -1569,7 +1577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
         <v>79668</v>
       </c>
@@ -1601,7 +1609,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
         <v>81594</v>
       </c>
@@ -1630,7 +1638,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
         <v>85291</v>
       </c>
@@ -1688,7 +1696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
         <v>87134</v>
       </c>
@@ -1717,7 +1725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
         <v>90553</v>
       </c>
@@ -1746,7 +1754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
         <v>90697</v>
       </c>
@@ -1775,7 +1783,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
         <v>92104</v>
       </c>
@@ -1804,7 +1812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
         <v>97700</v>
       </c>
@@ -1833,7 +1841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
         <v>97830</v>
       </c>
@@ -1862,7 +1870,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
         <v>102635</v>
       </c>
@@ -1891,7 +1899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2">
         <v>103834</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2">
         <v>107052</v>
       </c>
@@ -1949,7 +1957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
         <v>110829</v>
       </c>
@@ -1978,7 +1986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
         <v>110830</v>
       </c>
@@ -2020,10 +2028,10 @@
       <c r="D39" t="s">
         <v>47</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="10">
         <v>336</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="10" t="s">
         <v>48</v>
       </c>
       <c r="I39" t="s">
@@ -2036,7 +2044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2">
         <v>112214</v>
       </c>
@@ -2065,7 +2073,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
         <v>123539</v>
       </c>
@@ -2107,10 +2115,10 @@
       <c r="D42" t="s">
         <v>47</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="10">
         <v>348</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="10" t="s">
         <v>48</v>
       </c>
       <c r="I42" t="s">
@@ -2123,7 +2131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
         <v>133074</v>
       </c>
@@ -2152,7 +2160,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A44" s="2">
         <v>141566</v>
       </c>
@@ -2210,7 +2218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A46" s="2">
         <v>143787</v>
       </c>
@@ -2239,7 +2247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2">
         <v>143788</v>
       </c>
@@ -2271,7 +2279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2">
         <v>150598</v>
       </c>
@@ -2300,7 +2308,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2">
         <v>150599</v>
       </c>
@@ -2329,7 +2337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2">
         <v>150600</v>
       </c>
@@ -2358,7 +2366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A51" s="2">
         <v>152030</v>
       </c>
@@ -2387,7 +2395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A52" s="2">
         <v>163375</v>
       </c>
@@ -2416,7 +2424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A53" s="2">
         <v>168022</v>
       </c>
@@ -2445,7 +2453,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2">
         <v>168023</v>
       </c>
@@ -2474,7 +2482,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2">
         <v>168024</v>
       </c>
@@ -2506,7 +2514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
         <v>171209</v>
       </c>
@@ -2548,10 +2556,10 @@
       <c r="D57" t="s">
         <v>53</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="10">
         <v>456</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="10">
         <v>7.14</v>
       </c>
       <c r="I57" t="s">
@@ -2577,10 +2585,10 @@
       <c r="D58" t="s">
         <v>54</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="10">
         <v>456</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H58">
@@ -2596,7 +2604,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59" s="2">
         <v>200255</v>
       </c>
@@ -2625,7 +2633,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60" s="2">
         <v>201572</v>
       </c>
@@ -2654,7 +2662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A61" s="2">
         <v>201573</v>
       </c>
@@ -2683,7 +2691,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A62" s="2">
         <v>201574</v>
       </c>
@@ -2712,7 +2720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A63" s="2">
         <v>202962</v>
       </c>
@@ -2741,7 +2749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A64" s="2">
         <v>214716</v>
       </c>
@@ -2770,7 +2778,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2">
         <v>214717</v>
       </c>
@@ -2802,7 +2810,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="2">
         <v>218393</v>
       </c>
@@ -2832,7 +2840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A67" s="2">
         <v>218394</v>
       </c>
@@ -2877,7 +2885,7 @@
         <v>14.48</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A68" s="2">
         <v>218395</v>
       </c>
@@ -2918,7 +2926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2">
         <v>225059</v>
       </c>
@@ -2947,7 +2955,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A70" s="14">
         <v>225060</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A71" s="14">
         <v>225061</v>
       </c>
@@ -3011,7 +3019,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A72" s="14">
         <v>225062</v>
       </c>
@@ -3044,7 +3052,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A73" s="2">
         <v>230412</v>
       </c>
@@ -3073,7 +3081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A74" s="2">
         <v>230690</v>
       </c>
@@ -3131,7 +3139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A76" s="2">
         <v>245125</v>
       </c>
@@ -3160,7 +3168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A77" s="2">
         <v>246495</v>
       </c>
@@ -3189,7 +3197,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A78" s="2">
         <v>258361</v>
       </c>
@@ -3218,7 +3226,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A79" s="2">
         <v>258362</v>
       </c>
@@ -3250,7 +3258,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A80" s="2">
         <v>262138</v>
       </c>
@@ -3279,7 +3287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2">
         <v>262475</v>
       </c>
@@ -3308,7 +3316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="2">
         <v>274809</v>
       </c>
@@ -3337,7 +3345,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A83" s="2">
         <v>277104</v>
       </c>
@@ -3366,7 +3374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2">
         <v>281785</v>
       </c>
@@ -3395,7 +3403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2">
         <v>289924</v>
       </c>
@@ -3436,7 +3444,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N85" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}"/>
+  <autoFilter ref="A1:N85" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2eeac8d8feae4a8cad5a6af0499a211d"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="discount"/>
+        <filter val="#N/A"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N52">
     <sortCondition ref="N2:N52"/>
     <sortCondition ref="A2:A52"/>
@@ -3450,7 +3470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E05A46-80F6-40FB-B2FF-6933C154A4AB}">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">

</xml_diff>

<commit_message>
amount_of_compl and sum_rewards tested
</commit_message>
<xml_diff>
--- a/data/starbucks_data_test.xlsx
+++ b/data/starbucks_data_test.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADC1C3F0-C74B-4355-8AC5-0F83FF9D8E5F}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D118B291-D061-4BFD-9755-1BE53893BFB2}"/>
   <bookViews>
-    <workbookView xWindow="-27870" yWindow="0" windowWidth="13170" windowHeight="16200" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
   </bookViews>
   <sheets>
     <sheet name="transcript" sheetId="1" r:id="rId1"/>
@@ -861,9 +861,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -928,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>15561</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>47582</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>47583</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>49502</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>53176</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
         <v>53182</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
         <v>65844</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
         <v>85291</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2">
         <v>85293</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
         <v>87134</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
         <v>92104</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
         <v>110835</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2">
         <v>130152</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A44" s="2">
         <v>141566</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A45" s="2">
         <v>141567</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A48" s="2">
         <v>150598</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A52" s="2">
         <v>163375</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57" s="2">
         <v>187136</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58" s="2">
         <v>187137</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A60" s="2">
         <v>201572</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A66" s="2">
         <v>218393</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A67" s="2">
         <v>218394</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>14.48</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2">
         <v>218395</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A73" s="2">
         <v>230412</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A75" s="2">
         <v>243231</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A80" s="2">
         <v>262138</v>
       </c>
@@ -3447,13 +3447,7 @@
   <autoFilter ref="A1:N85" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
     <filterColumn colId="1">
       <filters>
-        <filter val="2eeac8d8feae4a8cad5a6af0499a211d"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="discount"/>
-        <filter val="#N/A"/>
+        <filter val="78afa995795e4d85b5d9ceeca43f5fef"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
offer_agg first complete run
</commit_message>
<xml_diff>
--- a/data/starbucks_data_test.xlsx
+++ b/data/starbucks_data_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FA7631E-7E9C-420B-9FE4-0B2C577F8E05}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B44DE8-CC6B-4777-97EE-07E64BC22355}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
     <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
   </bookViews>
   <sheets>
@@ -43,15 +43,31 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={822B2859-F0B3-401C-A49D-2534446F316C}</author>
+    <author>Balb, Oliver (FDS2)</author>
   </authors>
   <commentList>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{822B2859-F0B3-401C-A49D-2534446F316C}">
+    <comment ref="G46" authorId="0" shapeId="0" xr:uid="{487D7DBF-6A83-48D8-BD8C-33BC0EE67FE2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    offer not printed in update_offer_agg</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Balb, Oliver (FDS2):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wrong amount in offer_agg</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -133,9 +149,6 @@
     <t>2906b810c7d4411798c6938adc9daaa5</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>2eeac8d8feae4a8cad5a6af0499a211d</t>
   </si>
   <si>
@@ -277,9 +290,6 @@
     <t>ffff82501cea40309d5fdd7edcca4a07</t>
   </si>
   <si>
-    <t>of_dup</t>
-  </si>
-  <si>
     <t>{'amount': 16.06}</t>
   </si>
   <si>
@@ -359,13 +369,19 @@
   </si>
   <si>
     <t>offer_viewed_time_el</t>
+  </si>
+  <si>
+    <t>d-two-offers-same-completion-time</t>
+  </si>
+  <si>
+    <t>e-offer overlap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,6 +392,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -438,13 +455,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Porsche Next TT"/>
@@ -474,6 +484,53 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Porsche Next TT"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -541,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -568,16 +625,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,9 +656,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Balb, Oliver (FDS2)" id="{113F7940-6C74-4295-827D-8D05E1297FB4}" userId="Balb, Oliver (FDS2)" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,14 +954,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C12" dT="2024-11-22T09:19:23.82" personId="{113F7940-6C74-4295-827D-8D05E1297FB4}" id="{822B2859-F0B3-401C-A49D-2534446F316C}">
-    <text>offer not printed in update_offer_agg</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
   <sheetPr filterMode="1"/>
@@ -911,7 +961,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -929,12 +979,12 @@
     <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -961,16 +1011,16 @@
         <v>7</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>8</v>
@@ -1057,7 +1107,7 @@
         <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1065,28 +1115,28 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>28</v>
-      </c>
-      <c r="N5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
@@ -1094,19 +1144,19 @@
         <v>1393</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -1115,7 +1165,7 @@
         <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1126,7 +1176,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1155,7 +1205,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1181,19 +1231,19 @@
         <v>15836</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -1202,7 +1252,7 @@
         <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1213,7 +1263,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -1231,7 +1281,7 @@
         <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
@@ -1239,13 +1289,13 @@
         <v>32762</v>
       </c>
       <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
         <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>73</v>
       </c>
       <c r="E11">
         <v>60</v>
@@ -1260,7 +1310,7 @@
         <v>#N/A</v>
       </c>
       <c r="N11" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
@@ -1268,31 +1318,31 @@
         <v>32763</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
         <v>19</v>
       </c>
       <c r="N12" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
@@ -1300,13 +1350,13 @@
         <v>37060</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E13">
         <v>78</v>
@@ -1321,7 +1371,7 @@
         <v>#N/A</v>
       </c>
       <c r="N13" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
@@ -1329,13 +1379,13 @@
         <v>45575</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14">
         <v>120</v>
@@ -1350,7 +1400,7 @@
         <v>#N/A</v>
       </c>
       <c r="N14" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1361,10 +1411,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
       </c>
       <c r="E15">
         <v>132</v>
@@ -1390,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
       </c>
       <c r="E16">
         <v>132</v>
@@ -1405,7 +1455,7 @@
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" t="s">
         <v>13</v>
@@ -1430,10 +1480,10 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>144</v>
@@ -1462,19 +1512,19 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>168</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N18" t="s">
         <v>14</v>
@@ -1485,19 +1535,19 @@
         <v>53182</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19">
         <v>168</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>39</v>
+      <c r="F19" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
@@ -1506,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="N19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
@@ -1514,7 +1564,7 @@
         <v>54574</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1535,7 +1585,7 @@
         <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1543,19 +1593,19 @@
         <v>65844</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21">
         <v>168</v>
       </c>
-      <c r="F21" s="18" t="s">
-        <v>39</v>
+      <c r="F21" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="I21" t="s">
         <v>18</v>
@@ -1564,7 +1614,7 @@
         <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.4">
@@ -1572,10 +1622,10 @@
         <v>69626</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
@@ -1593,7 +1643,7 @@
         <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.4">
@@ -1601,13 +1651,13 @@
         <v>79667</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E23">
         <v>198</v>
@@ -1622,7 +1672,7 @@
         <v>#N/A</v>
       </c>
       <c r="N23" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.4">
@@ -1630,13 +1680,13 @@
         <v>79668</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24">
         <v>198</v>
@@ -1648,13 +1698,13 @@
         <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J24" t="s">
         <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.4">
@@ -1662,13 +1712,13 @@
         <v>81594</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E25">
         <v>204</v>
@@ -1683,7 +1733,7 @@
         <v>#N/A</v>
       </c>
       <c r="N25" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1694,22 +1744,22 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26">
         <v>216</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I26" t="s">
         <v>18</v>
       </c>
       <c r="J26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N26" t="s">
         <v>14</v>
@@ -1720,13 +1770,13 @@
         <v>85293</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27">
         <v>216</v>
@@ -1741,7 +1791,7 @@
         <v>#N/A</v>
       </c>
       <c r="N27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1752,10 +1802,10 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <v>222</v>
@@ -1781,10 +1831,10 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29">
         <v>234</v>
@@ -1807,13 +1857,13 @@
         <v>90697</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E30">
         <v>234</v>
@@ -1828,7 +1878,7 @@
         <v>#N/A</v>
       </c>
       <c r="N30" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1839,10 +1889,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31">
         <v>240</v>
@@ -1868,10 +1918,10 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32">
         <v>264</v>
@@ -1894,13 +1944,13 @@
         <v>97830</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E33">
         <v>264</v>
@@ -1915,7 +1965,7 @@
         <v>#N/A</v>
       </c>
       <c r="N33" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1926,10 +1976,10 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34">
         <v>288</v>
@@ -1944,7 +1994,7 @@
         <v>#N/A</v>
       </c>
       <c r="N34" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -1955,10 +2005,10 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35">
         <v>294</v>
@@ -1973,7 +2023,7 @@
         <v>#N/A</v>
       </c>
       <c r="N35" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.4">
@@ -1981,13 +2031,13 @@
         <v>107052</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E36">
         <v>312</v>
@@ -2002,7 +2052,7 @@
         <v>#N/A</v>
       </c>
       <c r="N36" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2016,19 +2066,19 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E37">
         <v>336</v>
       </c>
       <c r="F37" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" t="s">
         <v>27</v>
-      </c>
-      <c r="I37" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" t="s">
-        <v>28</v>
       </c>
       <c r="N37" t="s">
         <v>20</v>
@@ -2045,22 +2095,22 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E38">
         <v>336</v>
       </c>
       <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" t="s">
         <v>27</v>
       </c>
-      <c r="I38" t="s">
-        <v>18</v>
-      </c>
-      <c r="J38" t="s">
-        <v>28</v>
-      </c>
       <c r="N38" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2068,19 +2118,19 @@
         <v>110835</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="10">
         <v>336</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I39" t="s">
         <v>18</v>
@@ -2089,7 +2139,7 @@
         <v>19</v>
       </c>
       <c r="N39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.4">
@@ -2097,15 +2147,15 @@
         <v>112214</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="17">
         <v>336</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -2118,7 +2168,7 @@
         <v>19</v>
       </c>
       <c r="N40" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2129,22 +2179,22 @@
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E41">
         <v>336</v>
       </c>
       <c r="F41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" t="s">
         <v>27</v>
-      </c>
-      <c r="I41" t="s">
-        <v>18</v>
-      </c>
-      <c r="J41" t="s">
-        <v>28</v>
       </c>
       <c r="N41" t="s">
         <v>20</v>
@@ -2155,19 +2205,19 @@
         <v>130152</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" s="10">
         <v>348</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I42" t="s">
         <v>18</v>
@@ -2176,7 +2226,7 @@
         <v>19</v>
       </c>
       <c r="N42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.4">
@@ -2184,10 +2234,10 @@
         <v>133074</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -2205,7 +2255,7 @@
         <v>19</v>
       </c>
       <c r="N43" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2216,10 +2266,10 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E44">
         <v>378</v>
@@ -2242,13 +2292,13 @@
         <v>141567</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E45">
         <v>378</v>
@@ -2263,7 +2313,7 @@
         <v>#N/A</v>
       </c>
       <c r="N45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.4">
@@ -2271,18 +2321,18 @@
         <v>143787</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E46">
         <v>384</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="17">
         <v>15.57</v>
       </c>
       <c r="I46" t="s">
@@ -2292,39 +2342,39 @@
         <v>#N/A</v>
       </c>
       <c r="N46" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A47" s="19">
+      <c r="A47" s="18">
         <v>143788</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>33</v>
+        <v>70</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
-      </c>
-      <c r="E47">
+        <v>81</v>
+      </c>
+      <c r="E47" s="17">
         <v>384</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H47">
         <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J47" t="s">
         <v>19</v>
       </c>
       <c r="N47" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2338,13 +2388,13 @@
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48">
         <v>408</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I48" t="s">
         <v>18</v>
@@ -2367,19 +2417,19 @@
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E49">
         <v>408</v>
       </c>
       <c r="F49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I49" t="s">
         <v>18</v>
       </c>
       <c r="J49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N49" t="s">
         <v>20</v>
@@ -2389,19 +2439,19 @@
       <c r="A50" s="2">
         <v>150600</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="23">
         <v>408</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="23" t="s">
         <v>12</v>
       </c>
       <c r="I50" t="s">
@@ -2411,7 +2461,7 @@
         <v>13</v>
       </c>
       <c r="N50" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.4">
@@ -2419,18 +2469,18 @@
         <v>152030</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="10">
         <v>408</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="20" t="s">
         <v>23</v>
       </c>
       <c r="I51" t="s">
@@ -2440,7 +2490,7 @@
         <v>19</v>
       </c>
       <c r="N51" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2451,16 +2501,16 @@
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52">
         <v>408</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I52" t="s">
         <v>18</v>
@@ -2477,10 +2527,10 @@
         <v>168022</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -2498,7 +2548,7 @@
         <v>19</v>
       </c>
       <c r="N53" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.4">
@@ -2506,18 +2556,18 @@
         <v>168023</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E54">
         <v>414</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="10">
         <v>17.55</v>
       </c>
       <c r="I54" t="s">
@@ -2527,7 +2577,7 @@
         <v>#N/A</v>
       </c>
       <c r="N54" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.4">
@@ -2535,31 +2585,31 @@
         <v>168024</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>33</v>
+        <v>70</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
-      </c>
-      <c r="E55">
+        <v>81</v>
+      </c>
+      <c r="E55" s="10">
         <v>414</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H55">
         <v>2</v>
       </c>
       <c r="I55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J55" t="s">
         <v>19</v>
       </c>
       <c r="N55" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2570,7 +2620,7 @@
         <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -2588,7 +2638,7 @@
         <v>13</v>
       </c>
       <c r="N56" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2596,13 +2646,13 @@
         <v>187136</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E57" s="10">
         <v>456</v>
@@ -2617,7 +2667,7 @@
         <v>#N/A</v>
       </c>
       <c r="N57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2625,31 +2675,31 @@
         <v>187137</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E58" s="10">
         <v>456</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
       <c r="I58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J58" t="s">
         <v>19</v>
       </c>
       <c r="N58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.4">
@@ -2657,13 +2707,13 @@
         <v>200255</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E59">
         <v>498</v>
@@ -2678,7 +2728,7 @@
         <v>#N/A</v>
       </c>
       <c r="N59" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -2692,13 +2742,13 @@
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E60">
         <v>504</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I60" t="s">
         <v>18</v>
@@ -2743,20 +2793,20 @@
       <c r="A62" s="2">
         <v>201574</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="21" t="s">
         <v>10</v>
       </c>
       <c r="D62" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="21">
+        <v>504</v>
+      </c>
+      <c r="F62" s="21" t="s">
         <v>47</v>
-      </c>
-      <c r="E62">
-        <v>504</v>
-      </c>
-      <c r="F62" t="s">
-        <v>48</v>
       </c>
       <c r="I62" t="s">
         <v>18</v>
@@ -2765,7 +2815,7 @@
         <v>19</v>
       </c>
       <c r="N62" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.4">
@@ -2773,18 +2823,18 @@
         <v>202962</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="21" t="s">
         <v>10</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="21">
         <v>504</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="21" t="s">
         <v>12</v>
       </c>
       <c r="I63" t="s">
@@ -2794,7 +2844,7 @@
         <v>13</v>
       </c>
       <c r="N63" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.4">
@@ -2802,18 +2852,18 @@
         <v>214716</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E64">
         <v>504</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="21">
         <v>7.79</v>
       </c>
       <c r="I64" t="s">
@@ -2823,7 +2873,7 @@
         <v>#N/A</v>
       </c>
       <c r="N64" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.4">
@@ -2831,31 +2881,31 @@
         <v>214717</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" t="s">
         <v>33</v>
       </c>
-      <c r="D65" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65">
+      <c r="E65" s="21">
         <v>504</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="21" t="s">
         <v>12</v>
       </c>
       <c r="H65">
         <v>5</v>
       </c>
       <c r="I65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J65" t="s">
         <v>13</v>
       </c>
       <c r="N65" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
@@ -2866,10 +2916,10 @@
         <v>9</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E66" s="10">
         <v>510</v>
@@ -2896,23 +2946,23 @@
         <v>9</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E67" s="10">
         <v>510</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G67" s="10"/>
       <c r="H67" s="10">
         <v>10</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J67" s="10" t="s">
         <v>13</v>
@@ -2941,23 +2991,23 @@
         <v>9</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E68" s="10">
         <v>510</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G68" s="10"/>
       <c r="H68" s="10">
         <v>5</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>13</v>
@@ -2982,16 +3032,16 @@
         <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E69">
         <v>522</v>
       </c>
       <c r="F69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I69" t="s">
         <v>18</v>
@@ -3000,21 +3050,21 @@
         <v>19</v>
       </c>
       <c r="N69" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="14">
+      <c r="A70" s="2">
         <v>225060</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E70" s="10">
         <v>522</v>
@@ -3031,26 +3081,26 @@
         <v>#N/A</v>
       </c>
       <c r="N70" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="14">
+      <c r="A71" s="2">
         <v>225061</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="10">
+      <c r="E71" s="23">
         <v>522</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="F71" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G71" s="10"/>
@@ -3058,46 +3108,46 @@
         <v>5</v>
       </c>
       <c r="I71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J71" t="s">
         <v>13</v>
       </c>
       <c r="N71" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="14">
+      <c r="A72" s="2">
         <v>225062</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="11" t="s">
-        <v>33</v>
+      <c r="C72" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E72" s="10">
+        <v>53</v>
+      </c>
+      <c r="E72" s="21">
         <v>522</v>
       </c>
-      <c r="F72" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G72" s="10"/>
-      <c r="H72" s="10">
+      <c r="F72" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21">
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J72" t="s">
         <v>19</v>
       </c>
       <c r="N72" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
@@ -3108,10 +3158,10 @@
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E73">
         <v>534</v>
@@ -3134,10 +3184,10 @@
         <v>230690</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
@@ -3155,7 +3205,7 @@
         <v>13</v>
       </c>
       <c r="N74" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
@@ -3163,13 +3213,13 @@
         <v>243231</v>
       </c>
       <c r="B75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E75">
         <v>570</v>
@@ -3184,7 +3234,7 @@
         <v>#N/A</v>
       </c>
       <c r="N75" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
@@ -3221,7 +3271,7 @@
         <v>246495</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C77" t="s">
         <v>10</v>
@@ -3242,7 +3292,7 @@
         <v>19</v>
       </c>
       <c r="N77" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.4">
@@ -3250,13 +3300,13 @@
         <v>258361</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D78" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E78">
         <v>576</v>
@@ -3271,7 +3321,7 @@
         <v>#N/A</v>
       </c>
       <c r="N78" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.4">
@@ -3279,13 +3329,13 @@
         <v>258362</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E79">
         <v>576</v>
@@ -3297,13 +3347,13 @@
         <v>2</v>
       </c>
       <c r="I79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J79" t="s">
         <v>19</v>
       </c>
       <c r="N79" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
@@ -3314,16 +3364,16 @@
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E80">
         <v>582</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I80" t="s">
         <v>18</v>
@@ -3340,10 +3390,10 @@
         <v>262475</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D81" t="s">
         <v>22</v>
@@ -3361,7 +3411,7 @@
         <v>19</v>
       </c>
       <c r="N81" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.4">
@@ -3369,13 +3419,13 @@
         <v>274809</v>
       </c>
       <c r="B82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D82" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E82">
         <v>606</v>
@@ -3390,7 +3440,7 @@
         <v>#N/A</v>
       </c>
       <c r="N82" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
@@ -3401,10 +3451,10 @@
         <v>15</v>
       </c>
       <c r="C83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D83" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E83">
         <v>612</v>
@@ -3430,7 +3480,7 @@
         <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D84" t="s">
         <v>16</v>
@@ -3456,13 +3506,13 @@
         <v>289924</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D85" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E85">
         <v>648</v>
@@ -3477,25 +3527,25 @@
         <v>#N/A</v>
       </c>
       <c r="N85" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:14" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
       <c r="K88" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L88" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="L88" s="8" t="s">
+      <c r="M88" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="M88" s="8" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N85" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
-    <filterColumn colId="1">
+    <filterColumn colId="13">
       <filters>
-        <filter val="ffff82501cea40309d5fdd7edcca4a07"/>
+        <filter val="e-offer overlap"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3529,64 +3579,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="15" t="s">
-        <v>93</v>
+      <c r="A5" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="15" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="16" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successful test execution for offer_view_time calculation
</commit_message>
<xml_diff>
--- a/data/starbucks_data_test.xlsx
+++ b/data/starbucks_data_test.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B44DE8-CC6B-4777-97EE-07E64BC22355}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="8_{6B2006D7-1DB7-4FA1-BFA8-F3309D4F5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0EC410B-F1FD-444F-89AB-9A62C492BBDF}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
+    <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" xr2:uid="{9398EA58-2CD3-4D78-A8D1-C395CBD6642D}"/>
     <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" activeTab="1" xr2:uid="{59917EFC-C4A9-41F8-9FC6-0B56CABC658B}"/>
   </bookViews>
   <sheets>
     <sheet name="transcript" sheetId="1" r:id="rId1"/>
     <sheet name="transcript_agg" sheetId="2" r:id="rId2"/>
+    <sheet name="offer comp wo view" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">transcript!$A$1:$N$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">transcript!$A$2:$N$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
     <author>Balb, Oliver (FDS2)</author>
   </authors>
   <commentList>
-    <comment ref="G46" authorId="0" shapeId="0" xr:uid="{487D7DBF-6A83-48D8-BD8C-33BC0EE67FE2}">
+    <comment ref="G47" authorId="0" shapeId="0" xr:uid="{487D7DBF-6A83-48D8-BD8C-33BC0EE67FE2}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="104">
   <si>
     <t>person</t>
   </si>
@@ -375,13 +376,25 @@
   </si>
   <si>
     <t>e-offer overlap</t>
+  </si>
+  <si>
+    <t>offer_cmpl_time</t>
+  </si>
+  <si>
+    <t>offer_view_time</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>ok: offer viewed after offer completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,13 +507,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
       <name val="Porsche Next TT"/>
@@ -533,8 +539,46 @@
       <name val="Porsche Next TT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Porsche Next TT"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +600,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,10 +645,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -635,12 +686,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{488C8177-7084-4A8E-BCE3-DF0E3A1B267A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -653,10 +719,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -957,11 +1019,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O88"/>
+  <dimension ref="A2:O90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68:C69"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -979,126 +1041,101 @@
     <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2">
+      <c r="O2" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
+      <c r="F3" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -1107,143 +1144,143 @@
         <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
-        <v>1393</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>1393</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
         <v>15561</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2">
-        <v>15562</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
+      <c r="F8" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>15836</v>
+        <v>15562</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -1252,27 +1289,27 @@
         <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
-        <v>20283</v>
+        <v>15836</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
+        <v>46</v>
+      </c>
+      <c r="E10" s="28">
+        <v>6</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -1281,102 +1318,104 @@
         <v>19</v>
       </c>
       <c r="N10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2">
+        <v>20283</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="2">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2">
         <v>32762</v>
-      </c>
-      <c r="B11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11">
-        <v>60</v>
-      </c>
-      <c r="G11">
-        <v>16.059999999999999</v>
-      </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="2">
-        <v>32763</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>32</v>
+      <c r="C12" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12">
+        <v>71</v>
+      </c>
+      <c r="E12" s="28">
         <v>60</v>
       </c>
-      <c r="F12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28">
+        <v>16.059999999999999</v>
       </c>
       <c r="I12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J12" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
-        <v>37060</v>
+        <v>32763</v>
       </c>
       <c r="B13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="28">
+        <v>60</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13">
-        <v>78</v>
-      </c>
-      <c r="G13">
-        <v>7.18</v>
-      </c>
-      <c r="I13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" t="e">
-        <v>#N/A</v>
+      <c r="J13" t="s">
+        <v>19</v>
       </c>
       <c r="N13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
-        <v>45575</v>
+        <v>37060</v>
       </c>
       <c r="B14" t="s">
         <v>70</v>
@@ -1385,13 +1424,13 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="G14">
-        <v>9.1199999999999992</v>
+        <v>7.18</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -1403,24 +1442,24 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
-        <v>47582</v>
+        <v>45575</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E15">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G15">
-        <v>19.89</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1429,154 +1468,154 @@
         <v>#N/A</v>
       </c>
       <c r="N15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
-        <v>47583</v>
+        <v>47582</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>32</v>
+      <c r="C16" t="s">
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16">
         <v>132</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16">
-        <v>5</v>
+      <c r="G16">
+        <v>19.89</v>
       </c>
       <c r="I16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16">
-        <f>E16-E13</f>
-        <v>54</v>
-      </c>
-      <c r="L16">
-        <f>E16-E14</f>
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="J16" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
-        <v>49502</v>
+        <v>47583</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <v>132</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17">
-        <v>144</v>
-      </c>
-      <c r="G17">
-        <v>17.78</v>
-      </c>
-      <c r="I17" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" t="e">
-        <v>#N/A</v>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17">
+        <f>E17-E14</f>
+        <v>54</v>
+      </c>
+      <c r="L17">
+        <f>E17-E15</f>
+        <v>12</v>
       </c>
       <c r="N17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
-        <v>53176</v>
+        <v>49502</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18">
-        <v>168</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>36</v>
+        <v>144</v>
+      </c>
+      <c r="G18">
+        <v>17.78</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
-      <c r="J18" t="s">
-        <v>27</v>
+      <c r="J18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
-        <v>53182</v>
+        <v>53176</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>168</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>38</v>
+      <c r="F19" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="N19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
-        <v>54574</v>
+        <v>53182</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <v>168</v>
       </c>
-      <c r="F20" t="s">
-        <v>17</v>
+      <c r="F20" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
@@ -1585,28 +1624,29 @@
         <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
-        <v>65844</v>
+        <v>54574</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
+        <v>70</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="E21" s="30">
         <v>168</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F21" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="30"/>
       <c r="I21" t="s">
         <v>18</v>
       </c>
@@ -1614,27 +1654,27 @@
         <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
-        <v>69626</v>
+        <v>65844</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E22">
-        <v>174</v>
-      </c>
-      <c r="F22" t="s">
-        <v>17</v>
+        <v>168</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="I22" t="s">
         <v>18</v>
@@ -1643,94 +1683,97 @@
         <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
-        <v>79667</v>
+        <v>69626</v>
       </c>
       <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
-        <v>30</v>
+      <c r="C23" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23">
-        <v>198</v>
-      </c>
-      <c r="G23">
-        <v>22.88</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E23" s="30">
+        <v>174</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="30"/>
       <c r="I23" t="s">
         <v>18</v>
       </c>
-      <c r="J23" t="e">
-        <v>#N/A</v>
+      <c r="J23" t="s">
+        <v>19</v>
       </c>
       <c r="N23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
-        <v>79668</v>
+        <v>79667</v>
       </c>
       <c r="B24" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>32</v>
+      <c r="C24" s="30" t="s">
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24">
+        <v>74</v>
+      </c>
+      <c r="E24" s="30">
         <v>198</v>
       </c>
-      <c r="F24" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24">
-        <v>5</v>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30">
+        <v>22.88</v>
       </c>
       <c r="I24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J24" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
-        <v>81594</v>
+        <v>79668</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="30">
+        <v>198</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25" t="s">
         <v>30</v>
       </c>
-      <c r="D25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25">
-        <v>204</v>
-      </c>
-      <c r="G25">
-        <v>15.23</v>
-      </c>
-      <c r="I25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" t="e">
-        <v>#N/A</v>
+      <c r="J25" t="s">
+        <v>19</v>
       </c>
       <c r="N25" t="s">
         <v>99</v>
@@ -1738,80 +1781,80 @@
     </row>
     <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
+        <v>81594</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26">
+        <v>204</v>
+      </c>
+      <c r="G26">
+        <v>15.23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A27" s="2">
         <v>85291</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>29</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>35</v>
-      </c>
-      <c r="E26">
-        <v>216</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2">
-        <v>85293</v>
-      </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
       </c>
       <c r="E27">
         <v>216</v>
       </c>
-      <c r="G27">
-        <v>2.3199999999999998</v>
+      <c r="F27" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="I27" t="s">
         <v>18</v>
       </c>
-      <c r="J27" t="e">
-        <v>#N/A</v>
+      <c r="J27" t="s">
+        <v>27</v>
       </c>
       <c r="N27" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
-        <v>87134</v>
+        <v>85293</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G28">
-        <v>19.670000000000002</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="I28" t="s">
         <v>18</v>
@@ -1820,27 +1863,27 @@
         <v>#N/A</v>
       </c>
       <c r="N28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
-        <v>90553</v>
+        <v>87134</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G29">
-        <v>1.0900000000000001</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="I29" t="s">
         <v>18</v>
@@ -1849,27 +1892,27 @@
         <v>#N/A</v>
       </c>
       <c r="N29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
-        <v>90697</v>
+        <v>90553</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="E30">
         <v>234</v>
       </c>
       <c r="G30">
-        <v>18.079999999999998</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I30" t="s">
         <v>18</v>
@@ -1878,27 +1921,27 @@
         <v>#N/A</v>
       </c>
       <c r="N30" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
-        <v>92104</v>
+        <v>90697</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E31">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G31">
-        <v>29.72</v>
+        <v>18.079999999999998</v>
       </c>
       <c r="I31" t="s">
         <v>18</v>
@@ -1907,27 +1950,27 @@
         <v>#N/A</v>
       </c>
       <c r="N31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
-        <v>97700</v>
+        <v>92104</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="G32">
-        <v>3.5</v>
+        <v>29.72</v>
       </c>
       <c r="I32" t="s">
         <v>18</v>
@@ -1936,27 +1979,27 @@
         <v>#N/A</v>
       </c>
       <c r="N32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
-        <v>97830</v>
+        <v>97700</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="E33">
         <v>264</v>
       </c>
       <c r="G33">
-        <v>23.32</v>
+        <v>3.5</v>
       </c>
       <c r="I33" t="s">
         <v>18</v>
@@ -1965,27 +2008,27 @@
         <v>#N/A</v>
       </c>
       <c r="N33" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
-        <v>102635</v>
+        <v>97830</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="E34">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="G34">
-        <v>17.88</v>
+        <v>23.32</v>
       </c>
       <c r="I34" t="s">
         <v>18</v>
@@ -1994,12 +2037,12 @@
         <v>#N/A</v>
       </c>
       <c r="N34" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2">
-        <v>103834</v>
+        <v>102635</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -2008,13 +2051,13 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="G35">
-        <v>21.43</v>
+        <v>17.88</v>
       </c>
       <c r="I35" t="s">
         <v>18</v>
@@ -2026,24 +2069,24 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2">
-        <v>107052</v>
+        <v>103834</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="E36">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="G36">
-        <v>16.86</v>
+        <v>21.43</v>
       </c>
       <c r="I36" t="s">
         <v>18</v>
@@ -2052,44 +2095,44 @@
         <v>#N/A</v>
       </c>
       <c r="N36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
-        <v>110829</v>
+        <v>107052</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="E37">
-        <v>336</v>
-      </c>
-      <c r="F37" t="s">
-        <v>26</v>
+        <v>312</v>
+      </c>
+      <c r="G37">
+        <v>16.86</v>
       </c>
       <c r="I37" t="s">
         <v>18</v>
       </c>
-      <c r="J37" t="s">
-        <v>27</v>
+      <c r="J37" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N37" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
-        <v>110830</v>
+        <v>110829</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
@@ -2110,56 +2153,56 @@
         <v>27</v>
       </c>
       <c r="N38" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
-        <v>110835</v>
+        <v>110830</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
       </c>
       <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39">
+        <v>336</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" t="s">
+        <v>27</v>
+      </c>
+      <c r="N39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2">
+        <v>110835</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E40" s="10">
         <v>336</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="I39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" t="s">
-        <v>19</v>
-      </c>
-      <c r="N39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A40" s="2">
-        <v>112214</v>
-      </c>
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="17">
-        <v>336</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="I40" t="s">
         <v>18</v>
@@ -2168,85 +2211,85 @@
         <v>19</v>
       </c>
       <c r="N40" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
-        <v>123539</v>
+        <v>112214</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" t="s">
-        <v>29</v>
+        <v>70</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41">
+        <v>22</v>
+      </c>
+      <c r="E41" s="17">
         <v>336</v>
       </c>
-      <c r="F41" t="s">
-        <v>26</v>
+      <c r="F41" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="I41" t="s">
         <v>18</v>
       </c>
       <c r="J41" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="N41" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2">
-        <v>130152</v>
+        <v>123539</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="10">
-        <v>348</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="E42">
+        <v>336</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
       </c>
       <c r="I42" t="s">
         <v>18</v>
       </c>
       <c r="J42" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="N42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
-        <v>133074</v>
+        <v>130152</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43">
-        <v>354</v>
-      </c>
-      <c r="F43" t="s">
-        <v>23</v>
+        <v>46</v>
+      </c>
+      <c r="E43" s="10">
+        <v>348</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="I43" t="s">
         <v>18</v>
@@ -2255,56 +2298,56 @@
         <v>19</v>
       </c>
       <c r="N43" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A44" s="2">
+        <v>133074</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44">
+        <v>354</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s">
+        <v>19</v>
+      </c>
+      <c r="N44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
         <v>141566</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>9</v>
-      </c>
-      <c r="C44" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44">
-        <v>378</v>
-      </c>
-      <c r="G44">
-        <v>23.93</v>
-      </c>
-      <c r="I44" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="2">
-        <v>141567</v>
-      </c>
-      <c r="B45" t="s">
-        <v>24</v>
       </c>
       <c r="C45" t="s">
         <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45">
         <v>378</v>
       </c>
       <c r="G45">
-        <v>5.29</v>
+        <v>23.93</v>
       </c>
       <c r="I45" t="s">
         <v>18</v>
@@ -2313,27 +2356,27 @@
         <v>#N/A</v>
       </c>
       <c r="N45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A46" s="2">
-        <v>143787</v>
+        <v>141567</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="E46">
-        <v>384</v>
-      </c>
-      <c r="G46" s="17">
-        <v>15.57</v>
+        <v>378</v>
+      </c>
+      <c r="G46">
+        <v>5.29</v>
       </c>
       <c r="I46" t="s">
         <v>18</v>
@@ -2342,271 +2385,268 @@
         <v>#N/A</v>
       </c>
       <c r="N46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A47" s="18">
-        <v>143788</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2">
+        <v>143787</v>
       </c>
       <c r="B47" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="19" t="s">
-        <v>32</v>
+      <c r="C47" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="17">
+        <v>80</v>
+      </c>
+      <c r="E47">
         <v>384</v>
       </c>
-      <c r="F47" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47">
-        <v>2</v>
+      <c r="G47" s="17">
+        <v>15.57</v>
       </c>
       <c r="I47" t="s">
-        <v>30</v>
-      </c>
-      <c r="J47" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J47" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N47" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="2">
+      <c r="A48" s="18">
+        <v>143788</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="17">
+        <v>384</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>30</v>
+      </c>
+      <c r="J48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A49" s="2">
         <v>150598</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>9</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48">
-        <v>408</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I48" t="s">
-        <v>18</v>
-      </c>
-      <c r="J48" t="s">
-        <v>13</v>
-      </c>
-      <c r="N48" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="2">
-        <v>150599</v>
-      </c>
-      <c r="B49" t="s">
-        <v>15</v>
       </c>
       <c r="C49" t="s">
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E49">
         <v>408</v>
       </c>
-      <c r="F49" t="s">
-        <v>36</v>
+      <c r="F49" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="I49" t="s">
         <v>18</v>
       </c>
       <c r="J49" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="N49" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2">
+        <v>150599</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50">
+        <v>408</v>
+      </c>
+      <c r="F50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" t="s">
+        <v>27</v>
+      </c>
+      <c r="N50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2">
         <v>150600</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B51" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C51" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="23">
+      <c r="E51" s="22">
         <v>408</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F51" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I50" t="s">
-        <v>18</v>
-      </c>
-      <c r="J50" t="s">
+      <c r="I51" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" t="s">
         <v>13</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N51" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A51" s="2">
-        <v>152030</v>
-      </c>
-      <c r="B51" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" s="10">
-        <v>408</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" t="s">
-        <v>18</v>
-      </c>
-      <c r="J51" t="s">
-        <v>19</v>
-      </c>
-      <c r="N51" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A52" s="2">
-        <v>163375</v>
+        <v>152030</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>29</v>
+        <v>70</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52">
+        <v>22</v>
+      </c>
+      <c r="E52" s="10">
         <v>408</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>51</v>
+      <c r="F52" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I52" t="s">
         <v>18</v>
       </c>
       <c r="J52" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N52" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A53" s="2">
-        <v>168022</v>
+        <v>163375</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="E53">
-        <v>414</v>
-      </c>
-      <c r="F53" t="s">
-        <v>23</v>
+        <v>408</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="I53" t="s">
         <v>18</v>
       </c>
       <c r="J53" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N53" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2">
-        <v>168023</v>
+        <v>168022</v>
       </c>
       <c r="B54" t="s">
         <v>70</v>
       </c>
-      <c r="C54" t="s">
-        <v>30</v>
+      <c r="C54" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="E54">
         <v>414</v>
       </c>
-      <c r="G54" s="10">
-        <v>17.55</v>
+      <c r="F54" t="s">
+        <v>23</v>
       </c>
       <c r="I54" t="s">
         <v>18</v>
       </c>
-      <c r="J54" t="e">
-        <v>#N/A</v>
+      <c r="J54" t="s">
+        <v>19</v>
       </c>
       <c r="N54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2">
-        <v>168024</v>
+        <v>168023</v>
       </c>
       <c r="B55" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>32</v>
+      <c r="C55" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D55" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="10">
+        <v>82</v>
+      </c>
+      <c r="E55">
         <v>414</v>
       </c>
-      <c r="F55" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H55">
-        <v>2</v>
+      <c r="G55" s="10">
+        <v>17.55</v>
       </c>
       <c r="I55" t="s">
-        <v>30</v>
-      </c>
-      <c r="J55" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J55" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N55" t="s">
         <v>99</v>
@@ -2614,199 +2654,202 @@
     </row>
     <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
-        <v>171209</v>
+        <v>168024</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" t="s">
-        <v>29</v>
+        <v>70</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56">
-        <v>420</v>
-      </c>
-      <c r="F56" t="s">
-        <v>12</v>
+        <v>81</v>
+      </c>
+      <c r="E56" s="10">
+        <v>414</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
       </c>
       <c r="I56" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J56" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N56" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57" s="2">
-        <v>187136</v>
+        <v>171209</v>
       </c>
       <c r="B57" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>52</v>
-      </c>
-      <c r="E57" s="10">
-        <v>456</v>
-      </c>
-      <c r="G57" s="10">
-        <v>7.14</v>
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>420</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
       </c>
       <c r="I57" t="s">
         <v>18</v>
       </c>
-      <c r="J57" t="e">
-        <v>#N/A</v>
+      <c r="J57" t="s">
+        <v>13</v>
       </c>
       <c r="N57" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58" s="2">
-        <v>187137</v>
+        <v>187136</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>32</v>
+      <c r="C58" t="s">
+        <v>30</v>
       </c>
       <c r="D58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E58" s="10">
         <v>456</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H58">
-        <v>2</v>
+      <c r="G58" s="10">
+        <v>7.14</v>
       </c>
       <c r="I58" t="s">
-        <v>30</v>
-      </c>
-      <c r="J58" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J58" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N58" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59" s="2">
-        <v>200255</v>
+        <v>187137</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="10">
+        <v>456</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59" t="s">
         <v>30</v>
       </c>
-      <c r="D59" t="s">
-        <v>83</v>
-      </c>
-      <c r="E59">
-        <v>498</v>
-      </c>
-      <c r="G59">
-        <v>13.17</v>
-      </c>
-      <c r="I59" t="s">
-        <v>18</v>
-      </c>
-      <c r="J59" t="e">
-        <v>#N/A</v>
+      <c r="J59" t="s">
+        <v>19</v>
       </c>
       <c r="N59" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60" s="2">
+        <v>200255</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60">
+        <v>498</v>
+      </c>
+      <c r="G60">
+        <v>13.17</v>
+      </c>
+      <c r="I60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A61" s="2">
         <v>201572</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>9</v>
-      </c>
-      <c r="C60" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
-        <v>54</v>
-      </c>
-      <c r="E60">
-        <v>504</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I60" t="s">
-        <v>18</v>
-      </c>
-      <c r="J60" t="s">
-        <v>13</v>
-      </c>
-      <c r="N60" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="2">
-        <v>201573</v>
-      </c>
-      <c r="B61" t="s">
-        <v>15</v>
       </c>
       <c r="C61" t="s">
         <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="E61">
         <v>504</v>
       </c>
-      <c r="F61" t="s">
-        <v>17</v>
+      <c r="F61" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="I61" t="s">
         <v>18</v>
       </c>
       <c r="J61" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N61" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A62" s="2">
-        <v>201574</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C62" s="21" t="s">
+        <v>201573</v>
+      </c>
+      <c r="B62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" t="s">
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>46</v>
-      </c>
-      <c r="E62" s="21">
+        <v>16</v>
+      </c>
+      <c r="E62">
         <v>504</v>
       </c>
-      <c r="F62" s="21" t="s">
-        <v>47</v>
+      <c r="F62" t="s">
+        <v>17</v>
       </c>
       <c r="I62" t="s">
         <v>18</v>
@@ -2815,94 +2858,91 @@
         <v>19</v>
       </c>
       <c r="N62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2">
+        <v>201574</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="20">
+        <v>504</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" t="s">
+        <v>19</v>
+      </c>
+      <c r="N63" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A63" s="2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2">
         <v>202962</v>
-      </c>
-      <c r="B63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="21">
-        <v>504</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I63" t="s">
-        <v>18</v>
-      </c>
-      <c r="J63" t="s">
-        <v>13</v>
-      </c>
-      <c r="N63" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A64" s="2">
-        <v>214716</v>
       </c>
       <c r="B64" t="s">
         <v>70</v>
       </c>
-      <c r="C64" t="s">
-        <v>30</v>
+      <c r="C64" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>84</v>
-      </c>
-      <c r="E64">
+        <v>11</v>
+      </c>
+      <c r="E64" s="20">
         <v>504</v>
       </c>
-      <c r="G64" s="21">
-        <v>7.79</v>
+      <c r="F64" s="20" t="s">
+        <v>12</v>
       </c>
       <c r="I64" t="s">
         <v>18</v>
       </c>
-      <c r="J64" t="e">
-        <v>#N/A</v>
+      <c r="J64" t="s">
+        <v>13</v>
       </c>
       <c r="N64" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2">
-        <v>214717</v>
+        <v>214716</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="22" t="s">
-        <v>32</v>
+      <c r="C65" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>33</v>
-      </c>
-      <c r="E65" s="21">
+        <v>84</v>
+      </c>
+      <c r="E65">
         <v>504</v>
       </c>
-      <c r="F65" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H65">
-        <v>5</v>
+      <c r="G65" s="20">
+        <v>7.79</v>
       </c>
       <c r="I65" t="s">
-        <v>30</v>
-      </c>
-      <c r="J65" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="J65" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N65" t="s">
         <v>99</v>
@@ -2910,82 +2950,72 @@
     </row>
     <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="2">
+        <v>214717</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="20">
+        <v>504</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>30</v>
+      </c>
+      <c r="J66" t="s">
+        <v>13</v>
+      </c>
+      <c r="N66" t="s">
+        <v>99</v>
+      </c>
+      <c r="O66" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2">
         <v>218393</v>
-      </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E66" s="10">
-        <v>510</v>
-      </c>
-      <c r="G66" s="10">
-        <v>21.72</v>
-      </c>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N66" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="2">
-        <v>218394</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="11" t="s">
-        <v>32</v>
+      <c r="C67" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E67" s="10">
         <v>510</v>
       </c>
-      <c r="F67" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10">
-        <v>10</v>
-      </c>
+      <c r="G67" s="10">
+        <v>21.72</v>
+      </c>
+      <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J67" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K67">
-        <f>E67-E63</f>
-        <v>6</v>
-      </c>
-      <c r="L67">
-        <f>E67-E64</f>
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="J67" s="10" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N67" t="s">
         <v>14</v>
       </c>
-      <c r="O67">
-        <f>G66/15*10</f>
-        <v>14.48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A68" s="2">
-        <v>218395</v>
+        <v>218394</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
@@ -2994,91 +3024,104 @@
         <v>32</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E68" s="10">
         <v>510</v>
       </c>
-      <c r="F68" s="5" t="s">
-        <v>55</v>
+      <c r="F68" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="G68" s="10"/>
       <c r="H68" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>13</v>
       </c>
       <c r="K68">
+        <f>E68-E64</f>
+        <v>6</v>
+      </c>
+      <c r="L68">
         <f>E68-E65</f>
         <v>6</v>
       </c>
-      <c r="L68">
-        <f>E68-E70</f>
-        <v>-12</v>
-      </c>
       <c r="N68" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A69" s="2">
-        <v>225059</v>
+        <v>218395</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
-      </c>
-      <c r="C69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" t="s">
-        <v>46</v>
-      </c>
-      <c r="E69">
-        <v>522</v>
-      </c>
-      <c r="F69" t="s">
-        <v>47</v>
-      </c>
-      <c r="I69" t="s">
-        <v>18</v>
-      </c>
-      <c r="J69" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" s="10">
+        <v>510</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10">
+        <v>5</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69">
+        <f>E69-E66</f>
+        <v>6</v>
+      </c>
+      <c r="L69">
+        <f>E69-E71</f>
+        <v>-12</v>
       </c>
       <c r="N69" t="s">
-        <v>98</v>
+        <v>14</v>
+      </c>
+      <c r="O69" s="32" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A70" s="2">
-        <v>225060</v>
-      </c>
-      <c r="B70" s="10" t="s">
+        <v>225059</v>
+      </c>
+      <c r="B70" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E70" s="10">
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70">
         <v>522</v>
       </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="H70" s="10"/>
+      <c r="F70" t="s">
+        <v>47</v>
+      </c>
       <c r="I70" t="s">
         <v>18</v>
       </c>
-      <c r="J70" t="e">
-        <v>#N/A</v>
+      <c r="J70" t="s">
+        <v>19</v>
       </c>
       <c r="N70" t="s">
         <v>98</v>
@@ -3086,32 +3129,30 @@
     </row>
     <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A71" s="2">
-        <v>225061</v>
-      </c>
-      <c r="B71" s="23" t="s">
+        <v>225060</v>
+      </c>
+      <c r="B71" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="24" t="s">
-        <v>32</v>
+      <c r="C71" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E71" s="23">
+        <v>59</v>
+      </c>
+      <c r="E71" s="10">
         <v>522</v>
       </c>
-      <c r="F71" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10">
-        <v>5</v>
-      </c>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="H71" s="10"/>
       <c r="I71" t="s">
-        <v>30</v>
-      </c>
-      <c r="J71" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="J71" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N71" t="s">
         <v>98</v>
@@ -3119,32 +3160,32 @@
     </row>
     <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A72" s="2">
-        <v>225062</v>
-      </c>
-      <c r="B72" s="21" t="s">
+        <v>225061</v>
+      </c>
+      <c r="B72" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C72" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E72" s="21">
+        <v>33</v>
+      </c>
+      <c r="E72" s="22">
         <v>522</v>
       </c>
-      <c r="F72" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G72" s="21"/>
-      <c r="H72" s="21">
-        <v>2</v>
+      <c r="F72" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10">
+        <v>5</v>
       </c>
       <c r="I72" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J72" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N72" t="s">
         <v>98</v>
@@ -3152,138 +3193,142 @@
     </row>
     <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A73" s="2">
-        <v>230412</v>
-      </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" t="s">
-        <v>30</v>
-      </c>
-      <c r="D73" t="s">
-        <v>60</v>
-      </c>
-      <c r="E73">
-        <v>534</v>
-      </c>
-      <c r="G73">
-        <v>26.56</v>
+        <v>225062</v>
+      </c>
+      <c r="B73" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E73" s="20">
+        <v>522</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20">
+        <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" t="e">
-        <v>#N/A</v>
+        <v>32</v>
+      </c>
+      <c r="J73" t="s">
+        <v>19</v>
       </c>
       <c r="N73" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A74" s="2">
-        <v>230690</v>
+        <v>230412</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="E74">
         <v>534</v>
       </c>
-      <c r="F74" t="s">
-        <v>12</v>
+      <c r="G74">
+        <v>26.56</v>
       </c>
       <c r="I74" t="s">
         <v>18</v>
       </c>
-      <c r="J74" t="s">
-        <v>13</v>
+      <c r="J74" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N74" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A75" s="2">
-        <v>243231</v>
+        <v>230690</v>
       </c>
       <c r="B75" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75" t="s">
-        <v>30</v>
+        <v>70</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="D75" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E75">
-        <v>570</v>
-      </c>
-      <c r="G75">
-        <v>0.87</v>
+        <v>534</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>12</v>
       </c>
       <c r="I75" t="s">
         <v>18</v>
       </c>
-      <c r="J75" t="e">
-        <v>#N/A</v>
+      <c r="J75" t="s">
+        <v>13</v>
       </c>
       <c r="N75" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A76" s="2">
+        <v>243231</v>
+      </c>
+      <c r="B76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C76" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76">
+        <v>570</v>
+      </c>
+      <c r="G76">
+        <v>0.87</v>
+      </c>
+      <c r="I76" t="s">
+        <v>18</v>
+      </c>
+      <c r="J76" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="2">
         <v>245125</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>15</v>
-      </c>
-      <c r="C76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
-        <v>16</v>
-      </c>
-      <c r="E76">
-        <v>576</v>
-      </c>
-      <c r="F76" t="s">
-        <v>17</v>
-      </c>
-      <c r="I76" t="s">
-        <v>18</v>
-      </c>
-      <c r="J76" t="s">
-        <v>19</v>
-      </c>
-      <c r="N76" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A77" s="2">
-        <v>246495</v>
-      </c>
-      <c r="B77" t="s">
-        <v>70</v>
       </c>
       <c r="C77" t="s">
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E77">
         <v>576</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>23</v>
+      <c r="F77" t="s">
+        <v>17</v>
       </c>
       <c r="I77" t="s">
         <v>18</v>
@@ -3292,65 +3337,62 @@
         <v>19</v>
       </c>
       <c r="N77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A78" s="2">
-        <v>258361</v>
+        <v>246495</v>
       </c>
       <c r="B78" t="s">
         <v>70</v>
       </c>
-      <c r="C78" t="s">
-        <v>30</v>
+      <c r="C78" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="E78">
         <v>576</v>
       </c>
-      <c r="G78">
-        <v>14.23</v>
+      <c r="F78" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="I78" t="s">
         <v>18</v>
       </c>
-      <c r="J78" t="e">
-        <v>#N/A</v>
+      <c r="J78" t="s">
+        <v>19</v>
       </c>
       <c r="N78" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A79" s="2">
-        <v>258362</v>
+        <v>258361</v>
       </c>
       <c r="B79" t="s">
         <v>70</v>
       </c>
-      <c r="C79" s="12" t="s">
-        <v>32</v>
+      <c r="C79" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="D79" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E79">
         <v>576</v>
       </c>
-      <c r="F79" t="s">
-        <v>23</v>
-      </c>
-      <c r="H79">
-        <v>2</v>
+      <c r="G79" s="28">
+        <v>14.23</v>
       </c>
       <c r="I79" t="s">
-        <v>30</v>
-      </c>
-      <c r="J79" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J79" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N79" t="s">
         <v>99</v>
@@ -3358,86 +3400,92 @@
     </row>
     <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A80" s="2">
-        <v>262138</v>
+        <v>258362</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
-      </c>
-      <c r="C80" t="s">
-        <v>29</v>
+        <v>70</v>
+      </c>
+      <c r="C80" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="D80" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="E80">
-        <v>582</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>55</v>
+        <v>576</v>
+      </c>
+      <c r="F80" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80">
+        <v>2</v>
       </c>
       <c r="I80" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J80" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="N80" t="s">
-        <v>14</v>
+        <v>99</v>
+      </c>
+      <c r="O80" s="32" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A81" s="2">
-        <v>262475</v>
+        <v>262138</v>
       </c>
       <c r="B81" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
         <v>29</v>
       </c>
       <c r="D81" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="E81">
         <v>582</v>
       </c>
-      <c r="F81" t="s">
-        <v>23</v>
+      <c r="F81" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="I81" t="s">
         <v>18</v>
       </c>
       <c r="J81" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N81" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="2">
-        <v>274809</v>
+        <v>262475</v>
       </c>
       <c r="B82" t="s">
         <v>70</v>
       </c>
-      <c r="C82" t="s">
-        <v>30</v>
+      <c r="C82" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="D82" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="E82">
-        <v>606</v>
-      </c>
-      <c r="G82">
-        <v>10.119999999999999</v>
+        <v>582</v>
+      </c>
+      <c r="F82" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="I82" t="s">
         <v>18</v>
       </c>
-      <c r="J82" t="e">
-        <v>#N/A</v>
+      <c r="J82" t="s">
+        <v>19</v>
       </c>
       <c r="N82" t="s">
         <v>99</v>
@@ -3445,22 +3493,22 @@
     </row>
     <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A83" s="2">
-        <v>277104</v>
+        <v>274809</v>
       </c>
       <c r="B83" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
         <v>30</v>
       </c>
       <c r="D83" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E83">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="G83">
-        <v>0.06</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="I83" t="s">
         <v>18</v>
@@ -3469,89 +3517,124 @@
         <v>#N/A</v>
       </c>
       <c r="N83" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2">
-        <v>281785</v>
+        <v>277104</v>
       </c>
       <c r="B84" t="s">
         <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D84" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E84">
-        <v>624</v>
-      </c>
-      <c r="F84" t="s">
-        <v>17</v>
+        <v>612</v>
+      </c>
+      <c r="G84">
+        <v>0.06</v>
       </c>
       <c r="I84" t="s">
         <v>18</v>
       </c>
-      <c r="J84" t="s">
-        <v>19</v>
+      <c r="J84" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N84" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2">
+        <v>281785</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85">
+        <v>624</v>
+      </c>
+      <c r="F85" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" t="s">
+        <v>18</v>
+      </c>
+      <c r="J85" t="s">
+        <v>19</v>
+      </c>
+      <c r="N85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="2">
         <v>289924</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>70</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>30</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>87</v>
       </c>
-      <c r="E85">
+      <c r="E86">
         <v>648</v>
       </c>
-      <c r="G85">
+      <c r="G86">
         <v>18.91</v>
       </c>
-      <c r="I85" t="s">
-        <v>18</v>
-      </c>
-      <c r="J85" t="e">
+      <c r="I86" t="s">
+        <v>18</v>
+      </c>
+      <c r="J86" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N85" t="s">
+      <c r="N86" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="88" spans="1:14" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
-      <c r="K88" s="8" t="s">
+    <row r="89" spans="1:14" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
+      <c r="K89" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L88" s="8" t="s">
+      <c r="L89" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="M88" s="8" t="s">
+      <c r="M89" s="8" t="s">
         <v>69</v>
       </c>
     </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="F90">
+        <f>576-168</f>
+        <v>408</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N85" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
-    <filterColumn colId="13">
+  <autoFilter ref="A2:N86" xr:uid="{E9AEC0CB-C481-4D53-A8E1-9FB3A7338592}">
+    <filterColumn colId="1">
       <filters>
-        <filter val="e-offer overlap"/>
+        <filter val="78afa995795e4d85b5d9ceeca43f5fef"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N52">
-    <sortCondition ref="N2:N52"/>
-    <sortCondition ref="A2:A52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N53">
+    <sortCondition ref="N3:N53"/>
+    <sortCondition ref="A3:A53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3643,4 +3726,634 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02889C9C-11F9-43A5-9C8B-98C2253F4509}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" style="24" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="24">
+        <v>0</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="24">
+        <v>168</v>
+      </c>
+      <c r="G2" s="24">
+        <v>5</v>
+      </c>
+      <c r="H2" s="24">
+        <v>5</v>
+      </c>
+      <c r="I2" s="24">
+        <v>19.89</v>
+      </c>
+      <c r="J2" s="24">
+        <v>132</v>
+      </c>
+      <c r="K2" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="24">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="24">
+        <v>240</v>
+      </c>
+      <c r="G3" s="24">
+        <v>20</v>
+      </c>
+      <c r="H3" s="24">
+        <v>5</v>
+      </c>
+      <c r="K3" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="24">
+        <v>168</v>
+      </c>
+      <c r="G4" s="24">
+        <v>10</v>
+      </c>
+      <c r="H4" s="24">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>1393</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="24">
+        <v>240</v>
+      </c>
+      <c r="G5" s="24">
+        <v>10</v>
+      </c>
+      <c r="H5" s="24">
+        <v>2</v>
+      </c>
+      <c r="I5" s="24">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="J5" s="24">
+        <v>60</v>
+      </c>
+      <c r="K5" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>53182</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="24">
+        <v>168</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="24">
+        <v>168</v>
+      </c>
+      <c r="G6" s="24">
+        <v>7</v>
+      </c>
+      <c r="H6" s="24">
+        <v>3</v>
+      </c>
+      <c r="K6" s="24">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>54574</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="24">
+        <v>168</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="24">
+        <v>240</v>
+      </c>
+      <c r="G7" s="24">
+        <v>20</v>
+      </c>
+      <c r="H7" s="24">
+        <v>5</v>
+      </c>
+      <c r="I7" s="24">
+        <v>22.88</v>
+      </c>
+      <c r="J7" s="24">
+        <v>198</v>
+      </c>
+      <c r="K7" s="24">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>110835</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="24">
+        <v>336</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="24">
+        <v>240</v>
+      </c>
+      <c r="G8" s="24">
+        <v>10</v>
+      </c>
+      <c r="H8" s="24">
+        <v>2</v>
+      </c>
+      <c r="I8" s="24">
+        <v>7.14</v>
+      </c>
+      <c r="J8" s="24">
+        <v>456</v>
+      </c>
+      <c r="K8" s="24">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>112214</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="24">
+        <v>336</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="24">
+        <v>168</v>
+      </c>
+      <c r="G9" s="24">
+        <v>10</v>
+      </c>
+      <c r="H9" s="24">
+        <v>2</v>
+      </c>
+      <c r="I9" s="24">
+        <v>15.57</v>
+      </c>
+      <c r="J9" s="24">
+        <v>384</v>
+      </c>
+      <c r="K9" s="24">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>150598</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="24">
+        <v>408</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="24">
+        <v>168</v>
+      </c>
+      <c r="G10" s="24">
+        <v>10</v>
+      </c>
+      <c r="H10" s="24">
+        <v>10</v>
+      </c>
+      <c r="I10" s="24">
+        <v>14.48</v>
+      </c>
+      <c r="J10" s="24">
+        <v>510</v>
+      </c>
+      <c r="K10" s="24">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>150600</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="24">
+        <v>408</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="24">
+        <v>168</v>
+      </c>
+      <c r="G11" s="24">
+        <v>5</v>
+      </c>
+      <c r="H11" s="24">
+        <v>5</v>
+      </c>
+      <c r="I11" s="24">
+        <v>13.16</v>
+      </c>
+      <c r="J11" s="24">
+        <v>522</v>
+      </c>
+      <c r="K11" s="24">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>152030</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="24">
+        <v>408</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="24">
+        <v>168</v>
+      </c>
+      <c r="G12" s="24">
+        <v>10</v>
+      </c>
+      <c r="H12" s="24">
+        <v>2</v>
+      </c>
+      <c r="I12" s="24">
+        <v>17.55</v>
+      </c>
+      <c r="J12" s="24">
+        <v>414</v>
+      </c>
+      <c r="K12" s="24">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
+        <v>201572</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="24">
+        <v>504</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="24">
+        <v>120</v>
+      </c>
+      <c r="G13" s="24">
+        <v>5</v>
+      </c>
+      <c r="H13" s="24">
+        <v>5</v>
+      </c>
+      <c r="I13" s="24">
+        <v>7.24</v>
+      </c>
+      <c r="J13" s="24">
+        <v>510</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>201573</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="24">
+        <v>504</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="24">
+        <v>240</v>
+      </c>
+      <c r="G14" s="24">
+        <v>20</v>
+      </c>
+      <c r="H14" s="24">
+        <v>5</v>
+      </c>
+      <c r="K14" s="24">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>201574</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="24">
+        <v>504</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="24">
+        <v>240</v>
+      </c>
+      <c r="G15" s="24">
+        <v>10</v>
+      </c>
+      <c r="H15" s="24">
+        <v>2</v>
+      </c>
+      <c r="I15" s="24">
+        <v>5.26</v>
+      </c>
+      <c r="J15" s="24">
+        <v>522</v>
+      </c>
+      <c r="K15" s="24">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>202962</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="24">
+        <v>504</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="24">
+        <v>168</v>
+      </c>
+      <c r="G16" s="24">
+        <v>5</v>
+      </c>
+      <c r="H16" s="24">
+        <v>5</v>
+      </c>
+      <c r="I16" s="24">
+        <v>7.79</v>
+      </c>
+      <c r="J16" s="24">
+        <v>504</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>245125</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="24">
+        <v>576</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="24">
+        <v>240</v>
+      </c>
+      <c r="G17" s="24">
+        <v>20</v>
+      </c>
+      <c r="H17" s="24">
+        <v>5</v>
+      </c>
+      <c r="K17" s="24">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>246495</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="24">
+        <v>576</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="24">
+        <v>168</v>
+      </c>
+      <c r="G18" s="24">
+        <v>10</v>
+      </c>
+      <c r="H18" s="24">
+        <v>2</v>
+      </c>
+      <c r="I18" s="24">
+        <v>14.23</v>
+      </c>
+      <c r="J18" s="24">
+        <v>576</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>